<commit_message>
Allow multiple dataframe at the same line.
</commit_message>
<xml_diff>
--- a/pandaspy/testdata/dashboard_definition.xlsx
+++ b/pandaspy/testdata/dashboard_definition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="23040" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_cards" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>data card 1</t>
   </si>
@@ -24,7 +24,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>compound</t>
+    <t>compound query</t>
   </si>
   <si>
     <t>source 1</t>
@@ -75,12 +75,27 @@
     <t>data card 2</t>
   </si>
   <si>
+    <t>data card 3</t>
+  </si>
+  <si>
+    <t>other card</t>
+  </si>
+  <si>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>select sum(amount) as total_amount from plain;</t>
+  </si>
+  <si>
     <t xml:space="preserve">display card 1 based on data card 1 </t>
   </si>
   <si>
     <t>display card 2 based on data card 1</t>
   </si>
   <si>
+    <t>display card 6 based on data card 1</t>
+  </si>
+  <si>
     <t>column:num as Import Number</t>
   </si>
   <si>
@@ -97,6 +112,9 @@
   </si>
   <si>
     <t>column:email_address as Email</t>
+  </si>
+  <si>
+    <t>display card 5 based on data card 3</t>
   </si>
   <si>
     <t>display card 3 based on data card 2</t>
@@ -110,9 +128,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -132,6 +150,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -145,6 +170,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -152,34 +185,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,78 +255,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,25 +295,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,43 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,109 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,6 +500,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,8 +551,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,26 +586,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -576,145 +594,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1070,10 +1088,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1347,6 +1365,48 @@
         <v>17</v>
       </c>
     </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4">
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4">
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1357,13 +1417,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="23.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="33.5555555555556" customWidth="1"/>
@@ -1375,32 +1435,40 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4">
+      <c r="D8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1426,23 +1494,23 @@
   <sheetData>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>